<commit_message>
fixed path in excel files
</commit_message>
<xml_diff>
--- a/test/testcases/testcase28_manual_sql_notifications.xlsx
+++ b/test/testcases/testcase28_manual_sql_notifications.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\QE_ATF\test\testcases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\DATF_Other\Snowflake\QE_ATF\test\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B241CF7-7E32-4E5F-8CF6-883F71FD534A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE8D3CF-9120-4EE0-849C-E2CA9528E4F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -173,10 +173,10 @@
     <t>source_to_target</t>
   </si>
   <si>
-    <t>test\\sql\\targetsql</t>
-  </si>
-  <si>
-    <t>test\\sql\\sourcesql</t>
+    <t>test/sql/sourcesql</t>
+  </si>
+  <si>
+    <t>test/sql/targetsql</t>
   </si>
 </sst>
 </file>
@@ -572,7 +572,7 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,7 +689,7 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -781,7 +781,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>